<commit_message>
PROS-6604 - MARSRU - Development fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPI_Source.xlsx
+++ b/Projects/CCRU_SAND/Data/KPI_Source.xlsx
@@ -5,11 +5,20 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - FT" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Pos 2018 - MT - Convenience Big" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Pos 2018 - MT - Convenience Small" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Pos 2018 - MT - Hypermarket" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Pos 2018 - MT - Supermarket" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Pos 2018 - HoReCa - Bar Tavern Night Clubs" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Pos 2018 - HoReCa - Coffee Tea Shops" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Pos 2018 - HoReCa - Restaurant Cafe" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Pos 2018 - Canteen" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Pos 2018 - Petroleum" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Pos 2018 - QSR" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="60">
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
@@ -41,7 +50,7 @@
     <t xml:space="preserve">Pos 2018 - FT</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2018\FT PoS 2018.xlsx</t>
+    <t xml:space="preserve">KPIs_2018/FT PoS 2018.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">GAPS</t>
@@ -50,7 +59,7 @@
     <t xml:space="preserve">Top Gaps</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2018\gaps_guide_2018.xlsx</t>
+    <t xml:space="preserve">KPIs_2018/gaps_guide_2018.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">TARGET</t>
@@ -59,7 +68,7 @@
     <t xml:space="preserve">Target Execution 2018</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2018\Target Execution 2018.xlsx</t>
+    <t xml:space="preserve">KPIs_2018/Target Execution 2018.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">MARKETING</t>
@@ -68,7 +77,7 @@
     <t xml:space="preserve">Marketing 2017</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2018\Marketing.xlsx</t>
+    <t xml:space="preserve">KPIs_2018/Marketing.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">SPIRITS</t>
@@ -77,7 +86,7 @@
     <t xml:space="preserve">Spirits 2018 - FT</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2018\FT Spirits 2018.xlsx</t>
+    <t xml:space="preserve">KPIs_2018/FT Spirits 2018.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">CONTRACT</t>
@@ -86,7 +95,7 @@
     <t xml:space="preserve">Contract Execution</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2018\Contract Execution 2018.xlsx</t>
+    <t xml:space="preserve">KPIs_2018/Contract Execution 2018.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">EQUIPMENT</t>
@@ -107,7 +116,100 @@
     <t xml:space="preserve">Top SKU</t>
   </si>
   <si>
+    <t xml:space="preserve">KPI_CONVERTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Conversion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/KPIConversion.xlsx</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pos 2018 - MT - Convenience Big</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Convenience Big PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirits 2018 - MT - Convenience</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Convenience Spirits 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - MT - Convenience Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Convenience Small PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - MT - Hypermarket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Hypermarket PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Hypermarket Spirits 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - MT - Supermarket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Supermarket PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spirits 2018 - MT - Supermarket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Supermarket Spirits 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - HoReCa - Bar Tavern Night Clubs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/HoReCa Bar Tavern_Night Club PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - HoReCa Bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/HoReCa Spirits 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - HoReCa - Coffee Tea Shops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/HoReCa Cofee_Tea Shops PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - HoReCa Tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - HoReCa - Restaurant Cafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/HoReCa Restaurant_Cafe PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - Horeca cafe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - Canteen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Canteen PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - Petroleum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/Petroleum PoS 2018.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pos 2018 - QSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2018/QSR PoS 2018.xlsx</t>
   </si>
 </sst>
 </file>
@@ -140,19 +242,49 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11.5"/>
-      <color rgb="FFA5C261"/>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF33FF99"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66CCFF"/>
+        <bgColor rgb="FF9999FF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -189,12 +321,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,7 +380,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -245,13 +393,13 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FF66CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FFA5C261"/>
+      <rgbColor rgb="FF33FF99"/>
+      <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -275,32 +423,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -308,10 +456,10 @@
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -325,7 +473,7 @@
       <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -355,10 +503,10 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -372,7 +520,7 @@
       <c r="C7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -398,12 +546,315 @@
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -416,47 +867,47 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -466,8 +917,8 @@
       <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>28</v>
+      <c r="D3" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,14 +947,14 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -513,8 +964,8 @@
       <c r="C7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,10 +992,1079 @@
         <v>27</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
PROS-7196 - CCRU - Ext Planned Visits - Copy to SAND
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPI_Source.xlsx
+++ b/Projects/CCRU_SAND/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - FT" sheetId="1" state="hidden" r:id="rId2"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="123">
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
@@ -236,7 +236,7 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - FT - CAP.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2019/Gaps Guide 2018.xlsx</t>
+    <t xml:space="preserve">KPIs_2019/Gaps Guide 2019.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/Spirits 2018 - FT.xlsx</t>
@@ -299,6 +299,9 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub - CAP.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern CAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">KPIs_2019/Spirits 2018 - IC - HoReCa.xlsx</t>
   </si>
   <si>
@@ -311,16 +314,25 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub - REG.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern REG</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - CAP</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea - CAP.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS2019 ICHoReCa RestCafeTe CAP</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - REG</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea - REG.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS2019 ICHoReCa RestCafeTe REG</t>
   </si>
   <si>
     <t xml:space="preserve">PoS 2019 - IC Petroleum - CAP</t>
@@ -447,7 +459,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +494,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF99FFFF"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6666"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -519,7 +537,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -541,6 +559,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -576,7 +598,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FF99FFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6666"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
@@ -629,10 +651,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,10 +809,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -937,10 +961,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,17 +1107,16 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,7 +1155,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,11 +1234,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,7 +1276,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,11 +1355,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,7 +1397,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,11 +1476,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,7 +1518,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1576,11 +1597,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1619,7 +1639,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,11 +1742,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1765,7 +1784,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,16 +1882,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,8 +1928,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
+      <c r="D3" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1956,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,7 +1970,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1966,7 +1984,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2015,16 +2033,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,10 +2063,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2062,8 +2079,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
+      <c r="D3" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2107,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2121,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2118,7 +2135,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2172,10 +2189,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2324,16 +2342,15 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,10 +2372,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2371,8 +2388,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>51</v>
+      <c r="D3" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,7 +2416,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2413,7 +2430,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2427,7 +2444,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2475,17 +2492,16 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.8673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2507,10 +2523,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2523,8 +2539,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>51</v>
+      <c r="D3" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2551,7 +2567,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2565,7 +2581,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,7 +2595,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2633,10 +2649,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,10 +2675,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,7 +2692,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,7 +2727,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2724,7 +2741,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2778,10 +2795,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2803,10 +2821,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2820,7 +2838,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2855,7 +2873,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2869,7 +2887,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2923,10 +2941,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2948,10 +2967,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,7 +2984,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3000,7 +3019,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3014,7 +3033,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,10 +3087,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3093,10 +3113,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3110,7 +3130,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3137,7 +3157,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,7 +3171,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3165,7 +3185,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3219,10 +3239,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3244,10 +3265,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,7 +3282,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3288,7 +3309,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3302,7 +3323,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3316,7 +3337,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,10 +3391,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3395,10 +3417,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,7 +3434,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3439,7 +3461,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3453,7 +3475,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3467,7 +3489,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3521,10 +3543,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3546,10 +3569,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3563,7 +3586,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3590,7 +3613,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3604,7 +3627,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3618,7 +3641,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3672,10 +3695,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3697,10 +3721,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3714,7 +3738,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,7 +3765,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3755,7 +3779,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3769,7 +3793,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3823,10 +3847,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3980,10 +4005,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4005,10 +4031,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4022,7 +4048,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4049,7 +4075,7 @@
         <v>33</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4063,7 +4089,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4077,7 +4103,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4131,10 +4157,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4156,10 +4183,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4173,7 +4200,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4200,7 +4227,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4214,7 +4241,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4228,7 +4255,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4277,15 +4304,16 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4307,10 +4335,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4324,7 +4352,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4351,7 +4379,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4365,7 +4393,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4379,7 +4407,7 @@
         <v>74</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4433,10 +4461,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4590,10 +4619,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4747,10 +4777,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4904,10 +4935,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5061,10 +5093,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5218,10 +5251,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-10194 - CCRU Promo Tracking KPIs - copy PROD to SAND
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPI_Source.xlsx
+++ b/Projects/CCRU_SAND/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - FT" sheetId="1" state="hidden" r:id="rId2"/>
@@ -25,21 +25,26 @@
     <sheet name="PoS 2019 - FT NS - REG" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="PoS 2019 - IC Canteen - EDU" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="PoS 2019 - IC Canteen - OTH" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - CAP" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - REG" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - CAP" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - REG" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="PoS 2019 - IC Petroleum - CAP" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="PoS 2019 - IC Petroleum - REG" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="PoS 2019 - IC QSR" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="PoS 2019 - MT Conv Big - CAP" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="PoS 2019 - MT Conv Big - REG" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="PoS 2019 - MT Conv Small - CAP" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="PoS 2019 - MT Conv Small - REG" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="PoS 2019 - MT Hypermarket - CAP" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="PoS 2019 - MT Hypermarket - REG" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="PoS 2019 - MT Supermarket - CAP" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="PoS 2019 - MT Supermarket - REG" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - CAP" sheetId="19" state="hidden" r:id="rId20"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - REG" sheetId="20" state="hidden" r:id="rId21"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - CAP" sheetId="22" state="hidden" r:id="rId23"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - REG" sheetId="23" state="hidden" r:id="rId24"/>
+    <sheet name="PoS 2019 - IC Petroleum - CAP" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="PoS 2019 - IC Petroleum - REG" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="PoS 2019 - IC FastFood" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="PoS 2019 - IC QSR" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="PoS 2019 - IC Cinema - CAP" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="PoS 2019 - IC Cinema - REG" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="PoS 2019 - MT Conv Big - CAP" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="PoS 2019 - MT Conv Big - REG" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="PoS 2019 - MT Conv Small - CAP" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="PoS 2019 - MT Conv Small - REG" sheetId="33" state="visible" r:id="rId34"/>
+    <sheet name="PoS 2019 - MT Hypermarket - CAP" sheetId="34" state="visible" r:id="rId35"/>
+    <sheet name="PoS 2019 - MT Hypermarket - REG" sheetId="35" state="visible" r:id="rId36"/>
+    <sheet name="PoS 2019 - MT Supermarket - CAP" sheetId="36" state="visible" r:id="rId37"/>
+    <sheet name="PoS 2019 - MT Supermarket - REG" sheetId="37" state="visible" r:id="rId38"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="151">
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
@@ -317,6 +322,21 @@
     <t xml:space="preserve">Canteen OTH</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/Spirits 2018 - IC - HoReCa.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC - HoReCa ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoReCa</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - CAP</t>
   </si>
   <si>
@@ -326,15 +346,6 @@
     <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2019/Spirits 2018 - IC - HoReCa.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC - HoReCa All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoReCa</t>
-  </si>
-  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - REG</t>
   </si>
   <si>
@@ -344,6 +355,12 @@
     <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern REG</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea.xlsx</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - CAP</t>
   </si>
   <si>
@@ -380,16 +397,40 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Petroleum - REG.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC FastFood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC FastFood.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC - FastFood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FastFood</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC QSR</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC QSR.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">IC - QSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QSR</t>
+    <t xml:space="preserve">IC - QSR-Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR-Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Cinema - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Cinema - CAP.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Cinema - REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Cinema - REG.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">PoS 2019 - MT Conv Big - CAP</t>
@@ -719,10 +760,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,10 +919,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,10 +1071,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,17 +1217,16 @@
   </sheetPr>
   <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,11 +1359,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,11 +1495,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,11 +1631,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,11 +1767,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,11 +1926,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,16 +2080,15 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2127,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2154,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,7 +2168,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,7 +2182,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,7 +2212,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,21 +2240,21 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,10 +2276,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,7 +2293,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,7 +2320,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2334,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2348,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2378,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,10 +2416,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,6 +2564,7 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
@@ -2536,11 +2575,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,10 +2600,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,7 +2617,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,7 +2644,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,7 +2658,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,7 +2672,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,7 +2702,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,17 +2734,16 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,10 +2765,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2782,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,7 +2809,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,7 +2823,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,7 +2837,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2867,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,20 +2895,21 @@
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,10 +2931,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,7 +2947,7 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2933,6 +2971,12 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2945,7 +2989,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,7 +3003,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,7 +3033,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,20 +3061,21 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,10 +3097,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,8 +3113,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>107</v>
+      <c r="D3" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,6 +3137,12 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3104,7 +3155,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3118,7 +3169,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,7 +3199,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,10 +3237,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,10 +3263,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,7 +3280,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3315,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3277,7 +3329,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3359,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,10 +3397,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,10 +3423,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,7 +3440,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,12 +3463,6 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3428,7 +3475,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,7 +3489,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3519,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,15 +3552,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3535,10 +3583,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3552,7 +3600,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,14 +3623,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3593,10 +3635,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3607,7 +3649,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3626,7 +3668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -3637,7 +3679,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,15 +3712,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3700,10 +3743,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,7 +3760,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,14 +3783,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3758,10 +3795,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3772,7 +3809,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,7 +3828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -3835,15 +3872,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,10 +3903,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3882,7 +3920,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,14 +3943,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3923,10 +3955,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3937,7 +3969,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3956,7 +3988,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -3999,16 +4031,17 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,13 +4063,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -4047,7 +4080,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4070,14 +4103,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -4088,10 +4115,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -4102,7 +4129,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4121,7 +4148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -4132,7 +4159,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4170,10 +4197,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4327,10 +4355,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,10 +4381,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4369,7 +4398,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4393,7 +4422,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>127</v>
@@ -4492,10 +4521,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,10 +4547,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,7 +4564,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4558,10 +4588,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,7 +4649,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4657,10 +4687,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4682,10 +4713,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4699,7 +4730,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,10 +4754,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4784,7 +4815,837 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4822,10 +5683,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4979,10 +5841,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5136,10 +5999,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5293,10 +6157,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5450,10 +6315,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5607,10 +6473,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
CCRU - change log info to log debug - copy to SAND
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPI_Source.xlsx
+++ b/Projects/CCRU_SAND/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - FT" sheetId="1" state="hidden" r:id="rId2"/>
@@ -25,21 +25,26 @@
     <sheet name="PoS 2019 - FT NS - REG" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="PoS 2019 - IC Canteen - EDU" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="PoS 2019 - IC Canteen - OTH" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - CAP" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - REG" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - CAP" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - REG" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="PoS 2019 - IC Petroleum - CAP" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="PoS 2019 - IC Petroleum - REG" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="PoS 2019 - IC QSR" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="PoS 2019 - MT Conv Big - CAP" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="PoS 2019 - MT Conv Big - REG" sheetId="26" state="visible" r:id="rId27"/>
-    <sheet name="PoS 2019 - MT Conv Small - CAP" sheetId="27" state="visible" r:id="rId28"/>
-    <sheet name="PoS 2019 - MT Conv Small - REG" sheetId="28" state="visible" r:id="rId29"/>
-    <sheet name="PoS 2019 - MT Hypermarket - CAP" sheetId="29" state="visible" r:id="rId30"/>
-    <sheet name="PoS 2019 - MT Hypermarket - REG" sheetId="30" state="visible" r:id="rId31"/>
-    <sheet name="PoS 2019 - MT Supermarket - CAP" sheetId="31" state="visible" r:id="rId32"/>
-    <sheet name="PoS 2019 - MT Supermarket - REG" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - CAP" sheetId="19" state="hidden" r:id="rId20"/>
+    <sheet name="PoS 2019 - IC HoReCa BarTavernClub - REG" sheetId="20" state="hidden" r:id="rId21"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - CAP" sheetId="22" state="hidden" r:id="rId23"/>
+    <sheet name="PoS 2019 - IC HoReCa RestCafeTea - REG" sheetId="23" state="hidden" r:id="rId24"/>
+    <sheet name="PoS 2019 - IC Petroleum - CAP" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="PoS 2019 - IC Petroleum - REG" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="PoS 2019 - IC FastFood" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="PoS 2019 - IC QSR" sheetId="27" state="visible" r:id="rId28"/>
+    <sheet name="PoS 2019 - IC Cinema - CAP" sheetId="28" state="visible" r:id="rId29"/>
+    <sheet name="PoS 2019 - IC Cinema - REG" sheetId="29" state="visible" r:id="rId30"/>
+    <sheet name="PoS 2019 - MT Conv Big - CAP" sheetId="30" state="visible" r:id="rId31"/>
+    <sheet name="PoS 2019 - MT Conv Big - REG" sheetId="31" state="visible" r:id="rId32"/>
+    <sheet name="PoS 2019 - MT Conv Small - CAP" sheetId="32" state="visible" r:id="rId33"/>
+    <sheet name="PoS 2019 - MT Conv Small - REG" sheetId="33" state="visible" r:id="rId34"/>
+    <sheet name="PoS 2019 - MT Hypermarket - CAP" sheetId="34" state="visible" r:id="rId35"/>
+    <sheet name="PoS 2019 - MT Hypermarket - REG" sheetId="35" state="visible" r:id="rId36"/>
+    <sheet name="PoS 2019 - MT Supermarket - CAP" sheetId="36" state="visible" r:id="rId37"/>
+    <sheet name="PoS 2019 - MT Supermarket - REG" sheetId="37" state="visible" r:id="rId38"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="151">
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
@@ -317,6 +322,21 @@
     <t xml:space="preserve">Canteen OTH</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/Spirits 2018 - IC - HoReCa.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC - HoReCa ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HoReCa</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - CAP</t>
   </si>
   <si>
@@ -326,15 +346,6 @@
     <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">KPIs_2019/Spirits 2018 - IC - HoReCa.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC - HoReCa All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoReCa</t>
-  </si>
-  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa BarTavernClub - REG</t>
   </si>
   <si>
@@ -344,6 +355,12 @@
     <t xml:space="preserve">PoS 2019 ICHoReCa BarTavern REG</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC HoReCa RestCafeTea.xlsx</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC HoReCa RestCafeTea - CAP</t>
   </si>
   <si>
@@ -380,16 +397,40 @@
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Petroleum - REG.xlsx</t>
   </si>
   <si>
+    <t xml:space="preserve">PoS 2019 - IC FastFood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC FastFood.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC - FastFood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FastFood</t>
+  </si>
+  <si>
     <t xml:space="preserve">PoS 2019 - IC QSR</t>
   </si>
   <si>
     <t xml:space="preserve">KPIs_2019/PoS 2019 - IC QSR.xlsx</t>
   </si>
   <si>
-    <t xml:space="preserve">IC - QSR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QSR</t>
+    <t xml:space="preserve">IC - QSR-Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QSR-Cinema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Cinema - CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Cinema - CAP.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoS 2019 - IC Cinema - REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2019/PoS 2019 - IC Cinema - REG.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">PoS 2019 - MT Conv Big - CAP</t>
@@ -719,10 +760,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,10 +919,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,10 +1071,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,17 +1217,16 @@
   </sheetPr>
   <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,11 +1359,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,11 +1495,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,11 +1631,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1727,11 +1767,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,11 +1926,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,16 +2080,15 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2127,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2154,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,7 +2168,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,7 +2182,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2175,7 +2212,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2203,21 +2240,21 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="P33" activeCellId="0" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,10 +2276,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,7 +2293,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,7 +2320,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2334,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2348,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2378,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2379,10 +2416,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,6 +2564,7 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
@@ -2536,11 +2575,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,10 +2600,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,7 +2617,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2606,7 +2644,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,7 +2658,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,7 +2672,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2664,7 +2702,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,17 +2734,16 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.2755102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,10 +2765,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2782,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2772,7 +2809,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2786,7 +2823,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2800,7 +2837,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2830,7 +2867,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,20 +2895,21 @@
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2893,10 +2931,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,7 +2947,7 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="8" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2933,6 +2971,12 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -2945,7 +2989,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,7 +3003,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2989,7 +3033,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3017,20 +3061,21 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <tabColor rgb="FF333333"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,10 +3097,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3068,8 +3113,8 @@
       <c r="C3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>107</v>
+      <c r="D3" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,6 +3137,12 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3104,7 +3155,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3118,7 +3169,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3148,7 +3199,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3186,10 +3237,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3211,10 +3263,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,7 +3280,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3315,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3277,7 +3329,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3359,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3345,10 +3397,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3370,10 +3423,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3387,7 +3440,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3410,12 +3463,6 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3428,7 +3475,7 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3442,7 +3489,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3472,7 +3519,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3505,15 +3552,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3535,10 +3583,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3552,7 +3600,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3575,14 +3623,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3593,10 +3635,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3607,7 +3649,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3626,7 +3668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -3637,7 +3679,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3670,15 +3712,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3700,10 +3743,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,7 +3760,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3740,14 +3783,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3758,10 +3795,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3772,7 +3809,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,7 +3828,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -3835,15 +3872,16 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3865,10 +3903,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3882,7 +3920,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3905,14 +3943,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3923,10 +3955,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3937,7 +3969,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3956,7 +3988,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -3999,16 +4031,17 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,13 +4063,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -4047,7 +4080,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4070,14 +4103,8 @@
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -4088,10 +4115,10 @@
         <v>80</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -4102,7 +4129,7 @@
         <v>80</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4121,7 +4148,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>63</v>
       </c>
@@ -4132,7 +4159,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4170,10 +4197,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4327,10 +4355,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,10 +4381,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4369,7 +4398,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4393,7 +4422,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>127</v>
@@ -4492,10 +4521,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4517,10 +4547,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4534,7 +4564,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4558,10 +4588,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4619,7 +4649,7 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4657,10 +4687,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4682,10 +4713,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4699,7 +4730,7 @@
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4723,10 +4754,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4784,7 +4815,837 @@
         <v>65</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4822,10 +5683,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4979,10 +5841,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5136,10 +5999,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5293,10 +6157,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5450,10 +6315,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5607,10 +6473,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add targets to all pos sets
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPI_Source.xlsx
+++ b/Projects/CCRU_SAND/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="35"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="11" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="Pos 2018 - FT" sheetId="1" state="hidden" r:id="rId2"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="152">
   <si>
     <t xml:space="preserve">SOURCE</t>
   </si>
@@ -518,8 +518,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -551,7 +552,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -586,6 +587,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF99FFFF"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D18E"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -641,7 +648,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -666,7 +673,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -678,7 +693,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -707,7 +722,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFA9D18E"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -767,10 +782,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -925,10 +941,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,10 +1093,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,23 +1237,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E65536"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1248,11 +1266,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -1262,11 +1280,11 @@
       <c r="C2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="8" t="n">
         <v>65</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -1279,18 +1297,21 @@
       <c r="D3" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -1300,44 +1321,49 @@
       <c r="C6" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1346,7 +1372,6 @@
         <v>28</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1363,22 +1388,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65536"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1391,8 +1416,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -1402,8 +1430,11 @@
       <c r="C2" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -1417,17 +1448,17 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -1438,17 +1469,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -1456,27 +1488,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>67</v>
       </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1500,22 +1534,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65536"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1528,8 +1562,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -1539,8 +1576,11 @@
       <c r="C2" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -1554,17 +1594,17 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -1575,17 +1615,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -1593,27 +1634,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>72</v>
       </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1637,22 +1680,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D65536"/>
+  <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1665,8 +1708,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -1676,8 +1722,11 @@
       <c r="C2" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -1691,17 +1740,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -1712,17 +1761,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -1730,27 +1780,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>75</v>
       </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1774,22 +1826,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1802,8 +1854,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -1813,8 +1868,11 @@
       <c r="C2" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>78.7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -1828,7 +1886,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1839,17 +1897,17 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -1862,8 +1920,11 @@
       <c r="D7" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -1877,7 +1938,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -1885,29 +1946,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -1917,6 +1980,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1934,22 +1998,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1962,8 +2026,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -1973,8 +2040,11 @@
       <c r="C2" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>76.81</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -1987,8 +2057,9 @@
       <c r="D3" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -1998,18 +2069,21 @@
       <c r="C4" s="0" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -2022,8 +2096,11 @@
       <c r="D7" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -2036,38 +2113,42 @@
       <c r="D8" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -2077,6 +2158,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2094,22 +2176,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2122,8 +2204,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -2133,8 +2218,11 @@
       <c r="C2" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>77.73</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -2144,11 +2232,11 @@
       <c r="C3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -2159,12 +2247,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -2175,7 +2263,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -2188,8 +2276,11 @@
       <c r="D7" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -2203,7 +2294,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -2211,29 +2302,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -2243,6 +2336,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2269,11 +2363,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,7 +2405,7 @@
       <c r="C3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2393,10 +2487,10 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2435,10 +2529,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2593,11 +2688,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2635,7 +2730,7 @@
       <c r="C3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2717,10 +2812,10 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2751,22 +2846,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2779,8 +2874,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -2790,8 +2888,11 @@
       <c r="C2" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>75.66</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -2801,11 +2902,11 @@
       <c r="C3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -2816,12 +2917,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -2832,7 +2933,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -2845,8 +2946,11 @@
       <c r="D7" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -2860,7 +2964,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -2868,29 +2972,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -2900,6 +3006,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2926,11 +3033,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2968,7 +3075,7 @@
       <c r="C3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3050,10 +3157,10 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3093,11 +3200,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,7 +3242,7 @@
       <c r="C3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="11" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3217,10 +3324,10 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3251,21 +3358,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3278,8 +3386,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -3289,8 +3400,11 @@
       <c r="C2" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>63.36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -3304,7 +3418,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -3315,17 +3429,17 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3338,8 +3452,11 @@
       <c r="D7" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3353,7 +3470,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -3361,29 +3478,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -3393,6 +3512,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3410,21 +3530,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="6" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3437,8 +3559,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -3448,8 +3573,11 @@
       <c r="C2" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>63.36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -3462,8 +3590,9 @@
       <c r="D3" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -3473,18 +3602,21 @@
       <c r="C4" s="0" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -3497,8 +3629,11 @@
       <c r="D7" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -3511,38 +3646,41 @@
       <c r="D8" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -3569,21 +3707,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3596,8 +3735,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -3607,8 +3749,11 @@
       <c r="C2" s="3" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>80.33</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -3622,7 +3767,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -3633,12 +3778,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -3656,6 +3801,9 @@
       <c r="D7" s="2" t="s">
         <v>116</v>
       </c>
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -3671,7 +3819,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -3679,13 +3827,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -3694,14 +3843,15 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -3711,6 +3861,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3728,21 +3879,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3755,8 +3907,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -3766,8 +3921,11 @@
       <c r="C2" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>78.99</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -3781,7 +3939,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -3792,12 +3950,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -3815,6 +3973,7 @@
       <c r="D7" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -3830,7 +3989,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -3838,13 +3997,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -3853,14 +4013,15 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -3870,6 +4031,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3887,21 +4049,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3914,8 +4077,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -3925,8 +4091,11 @@
       <c r="C2" s="3" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>84.11</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -3939,8 +4108,9 @@
       <c r="D3" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -3950,16 +4120,19 @@
       <c r="C4" s="0" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -3974,6 +4147,9 @@
       <c r="D7" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -3988,22 +4164,25 @@
       <c r="D8" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -4012,14 +4191,15 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -4029,6 +4209,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4046,22 +4227,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4074,8 +4255,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -4084,6 +4268,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>125</v>
+      </c>
+      <c r="E2" s="8" t="n">
+        <v>83.34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4100,7 +4287,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -4111,12 +4298,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -4134,6 +4321,9 @@
       <c r="D7" s="2" t="s">
         <v>120</v>
       </c>
+      <c r="E7" s="8" t="n">
+        <v>95</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -4149,7 +4339,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -4157,13 +4347,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -4172,12 +4363,13 @@
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>121</v>
       </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -4214,10 +4406,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4363,21 +4556,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4390,8 +4584,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -4401,8 +4598,11 @@
       <c r="C2" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>70.71</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -4416,7 +4616,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -4427,12 +4627,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -4443,7 +4643,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -4456,8 +4656,11 @@
       <c r="D7" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -4471,7 +4674,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -4479,29 +4682,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -4511,6 +4718,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4528,21 +4736,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4555,8 +4764,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -4566,8 +4778,11 @@
       <c r="C2" s="3" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>73.8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -4581,7 +4796,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -4592,12 +4807,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -4608,7 +4823,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -4621,8 +4836,11 @@
       <c r="D7" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -4636,7 +4854,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -4644,27 +4862,31 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>133</v>
       </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -4693,21 +4915,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4720,8 +4943,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -4731,8 +4957,11 @@
       <c r="C2" s="3" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>70.7</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -4746,7 +4975,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -4757,12 +4986,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -4773,7 +5002,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -4786,8 +5015,11 @@
       <c r="D7" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -4801,7 +5033,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -4809,29 +5041,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -4841,6 +5077,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4858,21 +5095,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4885,8 +5123,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -4896,8 +5137,11 @@
       <c r="C2" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>69.52</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -4911,7 +5155,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -4922,12 +5166,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -4938,7 +5182,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -4951,8 +5195,11 @@
       <c r="D7" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -4966,7 +5213,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -4974,29 +5221,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -5006,6 +5257,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5023,21 +5275,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5050,8 +5303,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -5061,8 +5317,11 @@
       <c r="C2" s="3" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>65.15</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -5076,7 +5335,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -5087,12 +5346,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -5103,7 +5362,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -5116,8 +5375,11 @@
       <c r="D7" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -5131,7 +5393,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -5139,29 +5401,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -5171,6 +5437,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5188,21 +5455,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5215,8 +5483,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -5226,8 +5497,11 @@
       <c r="C2" s="3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>67.43</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -5241,7 +5515,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -5252,12 +5526,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -5268,7 +5542,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -5281,8 +5555,11 @@
       <c r="D7" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -5296,7 +5573,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -5304,29 +5581,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -5336,6 +5617,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5355,17 +5637,17 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9132653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5381,11 +5663,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -5395,11 +5677,11 @@
       <c r="C2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>67.3</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>66.35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -5413,7 +5695,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -5424,12 +5706,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -5440,7 +5722,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -5453,11 +5735,11 @@
       <c r="D7" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -5471,7 +5753,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
@@ -5479,32 +5761,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -5514,6 +5797,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5531,21 +5815,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5558,8 +5843,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E1" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>4</v>
       </c>
@@ -5569,8 +5857,11 @@
       <c r="C2" s="3" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="8" t="n">
+        <v>68.22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>7</v>
       </c>
@@ -5583,8 +5874,9 @@
       <c r="D3" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
@@ -5594,13 +5886,15 @@
       <c r="C4" s="0" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
@@ -5610,8 +5904,9 @@
       <c r="C6" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -5624,8 +5919,11 @@
       <c r="D7" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="8" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>22</v>
       </c>
@@ -5638,38 +5936,44 @@
       <c r="D8" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="8" t="n">
+        <v>95.8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
@@ -5679,6 +5983,7 @@
       <c r="C12" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="E12" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5704,10 +6009,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5861,10 +6167,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6018,10 +6325,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6175,10 +6483,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6332,10 +6641,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6489,10 +6799,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
copy code to sand, start coding
</commit_message>
<xml_diff>
--- a/Projects/CCRU_SAND/Data/KPI_Source.xlsx
+++ b/Projects/CCRU_SAND/Data/KPI_Source.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="POS" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,8 +17,9 @@
     <sheet name="KPI_CONVERSION" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="CONTRACT" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="SPIRITS" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="INTEGRATION" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="MARKETING" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="MARKETING" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="INTEGRATION" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="COOLER_AUDIT" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="236">
   <si>
     <t xml:space="preserve">POS</t>
   </si>
@@ -732,6 +733,12 @@
   </si>
   <si>
     <t xml:space="preserve">CCH Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COOLER_AUDIT_TOTAL_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPIs_2020/Cooler Quality 2020.xlsx</t>
   </si>
 </sst>
 </file>
@@ -847,7 +854,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -881,10 +888,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -972,20 +975,20 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2456,19 +2459,19 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,9 +2495,7 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
@@ -2503,9 +2504,7 @@
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
@@ -2514,9 +2513,7 @@
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
@@ -2525,9 +2522,7 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
@@ -2536,9 +2531,7 @@
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
@@ -2547,9 +2540,7 @@
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
@@ -2558,9 +2549,7 @@
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
@@ -2569,9 +2558,7 @@
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
@@ -2580,9 +2567,7 @@
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
@@ -2591,9 +2576,7 @@
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
@@ -2602,9 +2585,7 @@
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
@@ -2613,9 +2594,7 @@
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
@@ -2624,9 +2603,7 @@
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
@@ -2635,9 +2612,7 @@
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
@@ -2646,9 +2621,7 @@
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
@@ -2657,9 +2630,7 @@
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -2668,9 +2639,7 @@
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
@@ -2679,9 +2648,7 @@
       <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
@@ -2690,9 +2657,7 @@
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
@@ -2701,9 +2666,7 @@
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
@@ -2712,9 +2675,7 @@
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
@@ -2723,9 +2684,7 @@
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
@@ -2734,9 +2693,7 @@
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
@@ -2745,9 +2702,7 @@
       <c r="A25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
@@ -2756,9 +2711,7 @@
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
@@ -2767,9 +2720,7 @@
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>233</v>
-      </c>
+      <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
@@ -3049,19 +3000,19 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
+      <selection pane="bottomLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3085,7 +3036,9 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
@@ -3094,7 +3047,9 @@
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
@@ -3103,7 +3058,9 @@
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
@@ -3112,7 +3069,9 @@
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
@@ -3121,7 +3080,9 @@
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
@@ -3130,7 +3091,9 @@
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
@@ -3139,7 +3102,9 @@
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
@@ -3148,7 +3113,9 @@
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
@@ -3157,7 +3124,9 @@
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="5"/>
@@ -3166,7 +3135,9 @@
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="5"/>
@@ -3175,7 +3146,9 @@
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
@@ -3184,7 +3157,9 @@
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
@@ -3193,7 +3168,9 @@
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
@@ -3202,7 +3179,9 @@
       <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
@@ -3211,7 +3190,9 @@
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
@@ -3220,7 +3201,9 @@
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
@@ -3229,7 +3212,9 @@
       <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
@@ -3238,7 +3223,9 @@
       <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
@@ -3247,7 +3234,9 @@
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
@@ -3256,7 +3245,9 @@
       <c r="A21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
@@ -3265,7 +3256,9 @@
       <c r="A22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
@@ -3274,7 +3267,9 @@
       <c r="A23" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
@@ -3283,7 +3278,9 @@
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
@@ -3292,7 +3289,9 @@
       <c r="A25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
@@ -3301,7 +3300,9 @@
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
@@ -3310,7 +3311,9 @@
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
@@ -3568,6 +3571,1136 @@
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="s">
         <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFCC00"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E78"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D69" activeCellId="0" sqref="D69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.4534412955466"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3603238866397"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.0283400809717"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C69" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D71" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3589,19 +4722,19 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4292,12 +5425,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5341,19 +6474,19 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5699,10 +6832,10 @@
       <c r="A28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5710,10 +6843,10 @@
       <c r="A29" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5721,10 +6854,10 @@
       <c r="A30" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5732,10 +6865,10 @@
       <c r="A31" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5743,10 +6876,10 @@
       <c r="A32" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5754,10 +6887,10 @@
       <c r="A33" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5765,10 +6898,10 @@
       <c r="A34" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5776,10 +6909,10 @@
       <c r="A35" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5787,10 +6920,10 @@
       <c r="A36" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5798,10 +6931,10 @@
       <c r="A37" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5809,10 +6942,10 @@
       <c r="A38" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C38" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5820,10 +6953,10 @@
       <c r="A39" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5831,10 +6964,10 @@
       <c r="A40" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C40" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5842,10 +6975,10 @@
       <c r="A41" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C41" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5853,10 +6986,10 @@
       <c r="A42" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C42" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5864,10 +6997,10 @@
       <c r="A43" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5875,10 +7008,10 @@
       <c r="A44" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5886,10 +7019,10 @@
       <c r="A45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5897,10 +7030,10 @@
       <c r="A46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5908,10 +7041,10 @@
       <c r="A47" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5919,10 +7052,10 @@
       <c r="A48" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5930,10 +7063,10 @@
       <c r="A49" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5941,10 +7074,10 @@
       <c r="A50" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5952,10 +7085,10 @@
       <c r="A51" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5963,10 +7096,10 @@
       <c r="A52" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5974,10 +7107,10 @@
       <c r="A53" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5985,10 +7118,10 @@
       <c r="A54" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -5996,10 +7129,10 @@
       <c r="A55" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6007,10 +7140,10 @@
       <c r="A56" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6018,10 +7151,10 @@
       <c r="A57" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6029,10 +7162,10 @@
       <c r="A58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6040,10 +7173,10 @@
       <c r="A59" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6051,10 +7184,10 @@
       <c r="A60" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6062,10 +7195,10 @@
       <c r="A61" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6073,10 +7206,10 @@
       <c r="A62" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6084,10 +7217,10 @@
       <c r="A63" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6095,10 +7228,10 @@
       <c r="A64" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6106,10 +7239,10 @@
       <c r="A65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6117,10 +7250,10 @@
       <c r="A66" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6128,10 +7261,10 @@
       <c r="A67" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6139,10 +7272,10 @@
       <c r="A68" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B68" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C68" s="10" t="s">
+      <c r="C68" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6150,10 +7283,10 @@
       <c r="A69" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B69" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C69" s="10" t="s">
+      <c r="C69" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6161,10 +7294,10 @@
       <c r="A70" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="B70" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6172,10 +7305,10 @@
       <c r="A71" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="B71" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6183,10 +7316,10 @@
       <c r="A72" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B72" s="10" t="s">
+      <c r="B72" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C72" s="10" t="s">
+      <c r="C72" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6194,10 +7327,10 @@
       <c r="A73" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="B73" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C73" s="10" t="s">
+      <c r="C73" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6205,10 +7338,10 @@
       <c r="A74" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C74" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6216,10 +7349,10 @@
       <c r="A75" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="B75" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C75" s="10" t="s">
+      <c r="C75" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6227,10 +7360,10 @@
       <c r="A76" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="B76" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C76" s="10" t="s">
+      <c r="C76" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6238,10 +7371,10 @@
       <c r="A77" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B77" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C77" s="10" t="s">
+      <c r="C77" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6249,10 +7382,10 @@
       <c r="A78" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="B78" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="C78" s="10" t="s">
+      <c r="C78" s="9" t="s">
         <v>201</v>
       </c>
     </row>
@@ -6282,12 +7415,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6767,13 +7900,13 @@
       <c r="A43" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6781,13 +7914,13 @@
       <c r="A44" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6795,13 +7928,13 @@
       <c r="A45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6809,13 +7942,13 @@
       <c r="A46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6823,13 +7956,13 @@
       <c r="A47" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6837,13 +7970,13 @@
       <c r="A48" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6851,13 +7984,13 @@
       <c r="A49" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6865,13 +7998,13 @@
       <c r="A50" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6879,13 +8012,13 @@
       <c r="A51" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6893,13 +8026,13 @@
       <c r="A52" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="9" t="s">
         <v>209</v>
       </c>
     </row>
@@ -6907,13 +8040,13 @@
       <c r="A53" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6921,13 +8054,13 @@
       <c r="A54" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="9" t="s">
         <v>210</v>
       </c>
     </row>
@@ -6935,13 +8068,13 @@
       <c r="A55" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="9" t="s">
         <v>213</v>
       </c>
     </row>
@@ -6949,13 +8082,13 @@
       <c r="A56" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="9" t="s">
         <v>204</v>
       </c>
     </row>
@@ -6963,13 +8096,13 @@
       <c r="A57" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="9" t="s">
         <v>204</v>
       </c>
     </row>
@@ -6977,13 +8110,13 @@
       <c r="A58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="9" t="s">
         <v>214</v>
       </c>
     </row>
@@ -6991,13 +8124,13 @@
       <c r="A59" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="9" t="s">
         <v>213</v>
       </c>
     </row>
@@ -7005,13 +8138,13 @@
       <c r="A60" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="9" t="s">
         <v>215</v>
       </c>
     </row>
@@ -7019,13 +8152,13 @@
       <c r="A61" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="9" t="s">
         <v>206</v>
       </c>
     </row>
@@ -7033,13 +8166,13 @@
       <c r="A62" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="9" t="s">
         <v>208</v>
       </c>
     </row>
@@ -7047,13 +8180,13 @@
       <c r="A63" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D63" s="9" t="s">
         <v>208</v>
       </c>
     </row>
@@ -7061,13 +8194,13 @@
       <c r="A64" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="D64" s="9" t="s">
         <v>208</v>
       </c>
     </row>
@@ -7075,13 +8208,13 @@
       <c r="A65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="D65" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -7089,13 +8222,13 @@
       <c r="A66" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="D66" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -7103,13 +8236,13 @@
       <c r="A67" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" s="9" t="s">
         <v>216</v>
       </c>
     </row>
@@ -7209,19 +8342,19 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B42" activeCellId="0" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8020,20 +9153,20 @@
   </sheetPr>
   <dimension ref="A1:E65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8454,10 +9587,10 @@
       <c r="A43" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8465,10 +9598,10 @@
       <c r="A44" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8476,10 +9609,10 @@
       <c r="A45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8487,10 +9620,10 @@
       <c r="A46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8498,10 +9631,10 @@
       <c r="A47" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8509,10 +9642,10 @@
       <c r="A48" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8520,10 +9653,10 @@
       <c r="A49" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8531,10 +9664,10 @@
       <c r="A50" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8542,10 +9675,10 @@
       <c r="A51" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8553,10 +9686,10 @@
       <c r="A52" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8564,10 +9697,10 @@
       <c r="A53" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8575,10 +9708,10 @@
       <c r="A54" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8586,10 +9719,10 @@
       <c r="A55" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8597,10 +9730,10 @@
       <c r="A56" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8608,10 +9741,10 @@
       <c r="A57" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8619,10 +9752,10 @@
       <c r="A58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8630,10 +9763,10 @@
       <c r="A59" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8641,10 +9774,10 @@
       <c r="A60" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8652,10 +9785,10 @@
       <c r="A61" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8663,10 +9796,10 @@
       <c r="A62" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8674,10 +9807,10 @@
       <c r="A63" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8685,10 +9818,10 @@
       <c r="A64" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8696,10 +9829,10 @@
       <c r="A65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8707,10 +9840,10 @@
       <c r="A66" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8718,10 +9851,10 @@
       <c r="A67" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>220</v>
       </c>
     </row>
@@ -8832,19 +9965,19 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9373,13 +10506,13 @@
       <c r="A43" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E43" s="5" t="n">
@@ -9390,13 +10523,13 @@
       <c r="A44" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E44" s="5" t="n">
@@ -9407,13 +10540,13 @@
       <c r="A45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E45" s="5" t="n">
@@ -9424,13 +10557,13 @@
       <c r="A46" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E46" s="5" t="n">
@@ -9441,13 +10574,13 @@
       <c r="A47" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B47" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C47" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E47" s="5" t="n">
@@ -9458,13 +10591,13 @@
       <c r="A48" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E48" s="5" t="n">
@@ -9475,13 +10608,13 @@
       <c r="A49" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C49" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E49" s="5" t="n">
@@ -9492,13 +10625,13 @@
       <c r="A50" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E50" s="5" t="n">
@@ -9509,13 +10642,13 @@
       <c r="A51" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E51" s="5" t="n">
@@ -9526,13 +10659,13 @@
       <c r="A52" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C52" s="10" t="s">
+      <c r="C52" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="9" t="s">
         <v>209</v>
       </c>
       <c r="E52" s="5" t="n">
@@ -9543,13 +10676,13 @@
       <c r="A53" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C53" s="10" t="s">
+      <c r="C53" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E53" s="5" t="n">
@@ -9560,13 +10693,13 @@
       <c r="A54" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C54" s="10" t="s">
+      <c r="C54" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="9" t="s">
         <v>210</v>
       </c>
       <c r="E54" s="5" t="n">
@@ -9577,13 +10710,13 @@
       <c r="A55" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C55" s="10" t="s">
+      <c r="C55" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D55" s="9" t="s">
         <v>213</v>
       </c>
       <c r="E55" s="5" t="n">
@@ -9594,13 +10727,13 @@
       <c r="A56" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C56" s="10" t="s">
+      <c r="C56" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="9" t="s">
         <v>204</v>
       </c>
       <c r="E56" s="5" t="n">
@@ -9611,13 +10744,13 @@
       <c r="A57" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C57" s="10" t="s">
+      <c r="C57" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="9" t="s">
         <v>204</v>
       </c>
       <c r="E57" s="5" t="n">
@@ -9628,13 +10761,13 @@
       <c r="A58" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="9" t="s">
         <v>214</v>
       </c>
       <c r="E58" s="5" t="n">
@@ -9645,13 +10778,13 @@
       <c r="A59" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C59" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="9" t="s">
         <v>213</v>
       </c>
       <c r="E59" s="5" t="n">
@@ -9662,13 +10795,13 @@
       <c r="A60" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="9" t="s">
         <v>215</v>
       </c>
       <c r="E60" s="5" t="n">
@@ -9679,13 +10812,13 @@
       <c r="A61" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="9" t="s">
         <v>206</v>
       </c>
       <c r="E61" s="5" t="n">
@@ -9696,13 +10829,13 @@
       <c r="A62" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C62" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="9" t="s">
         <v>208</v>
       </c>
       <c r="E62" s="5" t="n">
@@ -9713,13 +10846,13 @@
       <c r="A63" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C63" s="10" t="s">
+      <c r="C63" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D63" s="10" t="s">
+      <c r="D63" s="9" t="s">
         <v>208</v>
       </c>
       <c r="E63" s="5" t="n">
@@ -9730,13 +10863,13 @@
       <c r="A64" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B64" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C64" s="10" t="s">
+      <c r="C64" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="D64" s="9" t="s">
         <v>208</v>
       </c>
       <c r="E64" s="5" t="n">
@@ -9747,13 +10880,13 @@
       <c r="A65" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C65" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D65" s="10" t="s">
+      <c r="D65" s="9" t="s">
         <v>216</v>
       </c>
       <c r="E65" s="5" t="n">
@@ -9764,13 +10897,13 @@
       <c r="A66" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C66" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="D66" s="9" t="s">
         <v>216</v>
       </c>
       <c r="E66" s="5" t="n">
@@ -9781,13 +10914,13 @@
       <c r="A67" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" s="9" t="s">
         <v>216</v>
       </c>
       <c r="E67" s="5" t="n">
@@ -9891,19 +11024,19 @@
   <dimension ref="A1:E65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B60" activeCellId="0" sqref="B60"/>
+      <selection pane="bottomLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.587044534413"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="55.417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1255060728745"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4534412955466"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8502024291498"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>